<commit_message>
2 new DOIs and work on issue 71 (registration form)
</commit_message>
<xml_diff>
--- a/metadata/rcs10/RLTLGRAIN/01-RothLTliming-grain.xlsx
+++ b/metadata/rcs10/RLTLGRAIN/01-RothLTliming-grain.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rothamsted.sharepoint.com/sites/e-RA/Shared Documents/General/Other long-term experiments/LT Liming expts/e-RA data/FAIRIFIED data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rothamsted.sharepoint.com/sites/e-RA/Shared Documents/Data-docs repository/metadata/rcs10/RLTLGRAIN/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CC9826E-B073-401C-A4F2-811F16267A6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{7CC9826E-B073-401C-A4F2-811F16267A6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D24C9802-9D2B-441F-9A9F-D1FA3463F6A0}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="-12555" windowWidth="19080" windowHeight="13965" xr2:uid="{5E827BFC-83F8-4F80-AE91-EA1F31D94EE5}"/>
+    <workbookView xWindow="1110" yWindow="-15480" windowWidth="19440" windowHeight="15000" xr2:uid="{5E827BFC-83F8-4F80-AE91-EA1F31D94EE5}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="6" r:id="rId1"/>
@@ -3247,14 +3247,14 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3289,7 +3289,7 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>5095875</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>181284</xdr:rowOff>
+      <xdr:rowOff>19359</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3631,8 +3631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB74C1FE-803F-443F-8178-861D574533BA}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3647,11 +3647,11 @@
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" ht="121.5" customHeight="1">
+    <row r="2" spans="1:3" ht="134.25" customHeight="1">
       <c r="A2" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="77" t="s">
         <v>128</v>
       </c>
       <c r="C2" s="20"/>
@@ -3838,19 +3838,19 @@
       <c r="A26" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="B26" s="77" t="s">
+      <c r="B26" s="78" t="s">
         <v>370</v>
       </c>
-      <c r="C26" s="77"/>
+      <c r="C26" s="78"/>
     </row>
     <row r="27" spans="1:3" ht="48" customHeight="1">
       <c r="A27" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="B27" s="78" t="s">
+      <c r="B27" s="79" t="s">
         <v>110</v>
       </c>
-      <c r="C27" s="78"/>
+      <c r="C27" s="79"/>
     </row>
     <row r="28" spans="1:3" ht="30.6" customHeight="1"/>
     <row r="29" spans="1:3" ht="30.6" customHeight="1">
@@ -17708,21 +17708,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100622C72A1DD75CA4D87E39FE37B04C3D3" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a181992610faed44b90126dc36e4bac8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6584b4ba-af75-4ac8-8379-7172592f8823" xmlns:ns3="a9e4a452-7199-439f-b4c2-3c6fe4528eb3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eb744a54a586913629e94f53228026f2" ns2:_="" ns3:_="">
     <xsd:import namespace="6584b4ba-af75-4ac8-8379-7172592f8823"/>
@@ -17939,32 +17924,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0809E8A-94F5-4669-8296-E1A8A89A2DCF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="6584b4ba-af75-4ac8-8379-7172592f8823"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a9e4a452-7199-439f-b4c2-3c6fe4528eb3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87EA80D3-49F4-411B-8D15-0F5A44EC82F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1CF841DE-FA6E-4BFD-8ED8-B3F46D9AA574}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17981,4 +17956,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87EA80D3-49F4-411B-8D15-0F5A44EC82F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0809E8A-94F5-4669-8296-E1A8A89A2DCF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="6584b4ba-af75-4ac8-8379-7172592f8823"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a9e4a452-7199-439f-b4c2-3c6fe4528eb3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>